<commit_message>
random during the calls
</commit_message>
<xml_diff>
--- a/04-English/EN3-work.xlsx
+++ b/04-English/EN3-work.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>too dire</t>
   </si>
@@ -62,9 +62,6 @@
     <t>connect to a windows server ?!</t>
   </si>
   <si>
-    <t>cli-skeleton (awscli)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mpi - message passing protocol </t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>Apache Spark is an open-source distributed general-purpose cluster-computing framework. Spark provides an interface for programming entire clusters with implicit data parallelism and fault tolerance. Originally developed at the University of California, Berkeley's AMPLab, the Spark codebase was later donated to the Apache Software Foundation, which has maintained it since.</t>
   </si>
   <si>
-    <t>bash scripting - TOPIC</t>
-  </si>
-  <si>
     <t>discontinued</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
   </si>
   <si>
     <t>SAM - TOPIC</t>
-  </si>
-  <si>
-    <t>ansible - TOPIC</t>
   </si>
   <si>
     <t>ITIL (Information Technolohy Infrastructure Library)</t>
@@ -234,13 +225,44 @@
     <t>the effective centre of an activity, region, or network.</t>
   </si>
   <si>
-    <t>monospace, non-proportional font</t>
-  </si>
-  <si>
     <t>facilitates</t>
   </si>
   <si>
     <t>megkonnyit</t>
+  </si>
+  <si>
+    <t>IBM Watson</t>
+  </si>
+  <si>
+    <t>Watson is a question-answering computer system capable of answering questions posed in natural language, developed in IBM's DeepQA project by a research team led by principal investigator David Ferrucci. Watson was named after IBM's first CEO, industrialist Thomas J. Watson</t>
+  </si>
+  <si>
+    <t>AWS CLI Skeletons</t>
+  </si>
+  <si>
+    <t>Most of the AWS Command Line Interface (AWS CLI) commands support the ability to accept all of the parameter input from a file using the --cli-input-json parameter.
+Those same commands helpfully provide the --generate-cli-skeleton to generate a file with all of the parameters that you can edit and fill in. Then you can run the command with the --cli-input-json parameter and point to the filled-in file. There are several AWS CLI commands that don't map directly to individual AWS API operations, such as the aws s3 commands. Such commands don't support either the --generate-cli-skeleton or --cli-input-json parameters that are discussed on this page.</t>
+  </si>
+  <si>
+    <t>Monospaced fonts</t>
+  </si>
+  <si>
+    <t>A monospaced font, also called a fixed-pitch, fixed-width, or non-proportional font, is a font whose letters and characters each occupy the same amount of horizontal space. This contrasts with variable-width fonts, where the letters and spacings have different widths.</t>
+  </si>
+  <si>
+    <t>MPI - Message Passing Interface</t>
+  </si>
+  <si>
+    <t>Message Passing Interface (MPI) is a standardized and portable message-passing standard designed by a group of researchers from academia and industry to function on a wide variety of parallel computing architectures. The standard defines the syntax and semantics of a core of library routines useful to a wide range of users writing portable message-passing programs in C, C++, and Fortran. There are several well-tested and efficient implementations of MPI, many of which are open-source or in the public domain. These fostered the development of a parallel software industry, and encouraged development of portable and scalable large-scale parallel applications.</t>
+  </si>
+  <si>
+    <t>foster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elosegit </t>
+  </si>
+  <si>
+    <t>encourage the development of (something, especially something desirable).</t>
   </si>
 </sst>
 </file>
@@ -313,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,9 +366,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálne" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -362,7 +387,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -651,17 +676,17 @@
   <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="82.28515625" customWidth="1"/>
-    <col min="2" max="2" width="63.28515625" customWidth="1"/>
+    <col min="1" max="1" width="82.33203125" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" customWidth="1"/>
     <col min="3" max="3" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -680,7 +705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -688,7 +713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -696,154 +721,165 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
         <v>59</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
         <v>61</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
         <v>63</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
         <v>65</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
         <v>69</v>
       </c>
-      <c r="B15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="3"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C104" s="3"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C105" s="2"/>
     </row>
-    <row r="106" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C110" s="2"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C111" s="2"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C112" s="2"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C113" s="2"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C114" s="2"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C115" s="2"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C116" s="2"/>
     </row>
   </sheetData>
@@ -854,296 +890,361 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
-    <col min="2" max="2" width="163.42578125" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="163.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="10"/>
+    </row>
+    <row r="18" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="11"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="11"/>
+    </row>
+    <row r="28" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="10"/>
+    </row>
+    <row r="33" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B33" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="10"/>
+    </row>
+    <row r="39" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B39" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="10"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="10"/>
+    </row>
+    <row r="44" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B44" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="10"/>
+    </row>
+    <row r="47" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B47" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="10"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="10"/>
+    </row>
+    <row r="51" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B51" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="52" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="10"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="10"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="10"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="10"/>
+    </row>
+    <row r="57" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B57" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="10"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="10"/>
+    </row>
+    <row r="62" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B62" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="10"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="10"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="10"/>
+    </row>
+    <row r="67" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B67" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="10"/>
-    </row>
-    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-    </row>
-    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-    </row>
-    <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
-    </row>
-    <row r="33" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-    </row>
-    <row r="39" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B39" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
-    </row>
-    <row r="44" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="10"/>
-    </row>
-    <row r="47" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B47" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="10"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="10"/>
-    </row>
-    <row r="51" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="10"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="10"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="10"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="10"/>
-    </row>
-    <row r="57" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="10"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="10"/>
-    </row>
-    <row r="62" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="10"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="10"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="10"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="10"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="10"/>
+    </row>
+    <row r="71" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B71" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="10"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="10"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="10"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="10"/>
+    </row>
+    <row r="77" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B77" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="10"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="10"/>
+    </row>
+    <row r="81" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B81" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="12"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="12"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="17">
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B82:B85"/>
     <mergeCell ref="B63:B66"/>
     <mergeCell ref="B52:B56"/>
     <mergeCell ref="B58:B60"/>

</xml_diff>

<commit_message>
addind tempalte which got deleted
</commit_message>
<xml_diff>
--- a/04-English/EN3-work.xlsx
+++ b/04-English/EN3-work.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>too dire</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>ITIL / ITSM</t>
-  </si>
-  <si>
-    <t>swagger</t>
   </si>
   <si>
     <t>connect to a windows server ?!</t>
@@ -383,6 +380,12 @@
     <t>Managed cloud services: AWS CloudFormation, CloudWatch, Lambdas, SQS, SNS, EC2, etc… or equivalents
 Linux, Git, infrastructure automation tools, scripting languages, monitoring tools (e.g. time series databases, log parsers, metric collectors, graphing tools, alerting tools)
 Java, PostgreSQL, Elasticsearch, Docker</t>
+  </si>
+  <si>
+    <t>swagger !!!</t>
+  </si>
+  <si>
+    <t>openAPI specification</t>
   </si>
 </sst>
 </file>
@@ -483,15 +486,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálne" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -507,7 +510,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -799,14 +802,14 @@
       <selection activeCell="C33" sqref="C33:C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="82.28515625" customWidth="1"/>
-    <col min="2" max="2" width="63.28515625" customWidth="1"/>
+    <col min="1" max="1" width="82.33203125" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" customWidth="1"/>
     <col min="3" max="3" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -817,7 +820,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -825,7 +828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -833,7 +836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -841,230 +844,230 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
         <v>50</v>
       </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>58</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>60</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>64</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>66</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="B16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" t="s">
         <v>78</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>79</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>81</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>83</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>85</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
         <v>87</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>89</v>
       </c>
-      <c r="C21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>90</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>92</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>93</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>95</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>96</v>
       </c>
-      <c r="C24" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="3"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C104" s="3"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C105" s="2"/>
     </row>
-    <row r="106" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C110" s="2"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C111" s="2"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C112" s="2"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C113" s="2"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C114" s="2"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C115" s="2"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C116" s="2"/>
     </row>
   </sheetData>
@@ -1077,363 +1080,363 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
-    <col min="2" max="2" width="163.42578125" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="163.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="10"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="10"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" s="10"/>
+    </row>
+    <row r="18" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="12"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="12"/>
+    </row>
+    <row r="28" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="10"/>
+    </row>
+    <row r="33" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B33" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="10"/>
+    </row>
+    <row r="39" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B39" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="10"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="10"/>
+    </row>
+    <row r="44" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B44" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="10"/>
+    </row>
+    <row r="47" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B47" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="10"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="10"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="10"/>
-    </row>
-    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-    </row>
-    <row r="18" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-    </row>
-    <row r="22" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-    </row>
-    <row r="28" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
-    </row>
-    <row r="33" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-    </row>
-    <row r="39" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B39" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
-    </row>
-    <row r="44" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="10"/>
-    </row>
-    <row r="47" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B47" s="5" t="s">
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="10" t="s">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="10"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="10"/>
+    </row>
+    <row r="51" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B51" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="10"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="10"/>
-    </row>
-    <row r="51" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="9" t="s">
+    <row r="52" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" s="10"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="10"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="10"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="10"/>
     </row>
-    <row r="57" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" ht="18" x14ac:dyDescent="0.3">
       <c r="B57" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="10" t="s">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="10"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="10"/>
+    </row>
+    <row r="62" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B62" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="10"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="10"/>
-    </row>
-    <row r="62" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="9" t="s">
+    <row r="63" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="10"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="10"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="10"/>
     </row>
-    <row r="67" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B67" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="10" t="s">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="10"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="10"/>
+    </row>
+    <row r="71" spans="2:2" ht="18" x14ac:dyDescent="0.3">
+      <c r="B71" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="10"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="10"/>
-    </row>
-    <row r="71" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B71" s="9" t="s">
+    <row r="72" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="10" t="s">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="10"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="10"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="10"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="10"/>
+    </row>
+    <row r="77" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B77" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="10"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="10"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="10"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="10"/>
-    </row>
-    <row r="77" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B77" s="5" t="s">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="10" t="s">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="10"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="10"/>
+    </row>
+    <row r="81" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B81" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="10"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="10"/>
-    </row>
-    <row r="81" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B81" s="5" t="s">
+    <row r="82" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="12"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="12"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="12"/>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="11"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="11"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B63:B66"/>
     <mergeCell ref="B52:B56"/>
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="B2:B5"/>
@@ -1446,6 +1449,11 @@
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B63:B66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1456,116 +1464,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="88.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+    <col min="2" max="2" width="88.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" t="s">
         <v>102</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" t="s">
         <v>104</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B5" t="s">
         <v>106</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B6" t="s">
         <v>108</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B7" t="s">
         <v>110</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B8" t="s">
         <v>112</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B9" t="s">
         <v>114</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B10" t="s">
         <v>116</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ml-la pract. exam 78%
</commit_message>
<xml_diff>
--- a/04-English/EN3-work.xlsx
+++ b/04-English/EN3-work.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
   <si>
     <t>too dire</t>
   </si>
@@ -437,6 +437,27 @@
   </si>
   <si>
     <t>szoras</t>
+  </si>
+  <si>
+    <t>corpus</t>
+  </si>
+  <si>
+    <t>gyujtemeny</t>
+  </si>
+  <si>
+    <t>fraction</t>
+  </si>
+  <si>
+    <t>toredek</t>
+  </si>
+  <si>
+    <t>impute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">betud, berak, </t>
+  </si>
+  <si>
+    <t>impute values for missing data</t>
   </si>
 </sst>
 </file>
@@ -537,11 +558,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -849,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,6 +1118,33 @@
       </c>
       <c r="B28" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
@@ -1296,7 +1344,7 @@
       <c r="A19" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1304,13 +1352,13 @@
       <c r="A20" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="11"/>
+      <c r="B20" s="12"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>130</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="12"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1321,18 +1369,18 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
+      <c r="B24" s="12"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
+      <c r="B25" s="12"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
+      <c r="B26" s="12"/>
     </row>
     <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
@@ -1534,26 +1582,21 @@
       </c>
     </row>
     <row r="82" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="12" t="s">
+      <c r="B82" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="12"/>
+      <c r="B83" s="11"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="12"/>
+      <c r="B84" s="11"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="12"/>
+      <c r="B85" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B63:B66"/>
     <mergeCell ref="B52:B56"/>
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="B2:B5"/>
@@ -1566,6 +1609,11 @@
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B63:B66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ml, la practice test
</commit_message>
<xml_diff>
--- a/04-English/EN3-work.xlsx
+++ b/04-English/EN3-work.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>too dire</t>
   </si>
@@ -458,6 +458,21 @@
   </si>
   <si>
     <t>impute values for missing data</t>
+  </si>
+  <si>
+    <t>pecularities</t>
+  </si>
+  <si>
+    <t>sajatossagok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pecularities of the training data… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fine print </t>
+  </si>
+  <si>
+    <t>text in a formal agreement that is printed smaller than the rest of the text, sometimes in the hope that it will not be noticed</t>
   </si>
 </sst>
 </file>
@@ -566,7 +581,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálne" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -582,7 +597,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -870,18 +885,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="82.28515625" customWidth="1"/>
-    <col min="2" max="2" width="63.28515625" customWidth="1"/>
+    <col min="1" max="1" width="82.33203125" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" customWidth="1"/>
     <col min="3" max="3" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -892,7 +907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -900,7 +915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -908,7 +923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -916,7 +931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -924,7 +939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -932,7 +947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -940,7 +955,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -948,7 +963,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -956,7 +971,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -964,7 +979,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -972,7 +987,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -980,7 +995,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -988,7 +1003,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -996,7 +1011,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1004,7 +1019,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1012,7 +1027,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -1023,7 +1038,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -1031,7 +1046,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>82</v>
       </c>
@@ -1039,7 +1054,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>84</v>
       </c>
@@ -1047,7 +1062,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -1058,7 +1073,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>89</v>
       </c>
@@ -1066,7 +1081,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>91</v>
       </c>
@@ -1077,7 +1092,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1088,7 +1103,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -1096,7 +1111,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -1104,7 +1119,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>134</v>
       </c>
@@ -1112,7 +1127,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>136</v>
       </c>
@@ -1120,7 +1135,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -1128,7 +1143,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>140</v>
       </c>
@@ -1136,7 +1151,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>142</v>
       </c>
@@ -1147,58 +1162,77 @@
         <v>144</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" s="3"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" s="3"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" s="3"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" s="3"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C104" s="3"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C105" s="2"/>
     </row>
-    <row r="106" spans="3:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C106" s="4"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C107" s="1"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C108" s="1"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C109" s="1"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C110" s="2"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C111" s="2"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C112" s="2"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C113" s="2"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C114" s="2"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C115" s="2"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C116" s="2"/>
     </row>
   </sheetData>
@@ -1215,13 +1249,13 @@
       <selection activeCell="B19" sqref="B19:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
-    <col min="2" max="2" width="163.42578125" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="163.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
@@ -1229,7 +1263,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1237,30 +1271,30 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1268,7 +1302,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1276,36 +1310,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>119</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -1313,7 +1347,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -1321,18 +1355,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>123</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -1340,7 +1374,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -1348,19 +1382,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>129</v>
       </c>
       <c r="B20" s="12"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>130</v>
       </c>
       <c r="B21" s="12"/>
     </row>
-    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -1368,231 +1402,231 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26" s="12"/>
     </row>
-    <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B29" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B31" s="10"/>
     </row>
-    <row r="33" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" ht="18" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="10"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="10"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="10"/>
     </row>
-    <row r="39" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B39" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="10"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="10"/>
     </row>
-    <row r="44" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" ht="18" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="2:2" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="10"/>
     </row>
-    <row r="47" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B47" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="10"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" s="10"/>
     </row>
-    <row r="51" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" ht="18" x14ac:dyDescent="0.3">
       <c r="B51" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" s="10"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="10"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="10"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="10"/>
     </row>
-    <row r="57" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" ht="18" x14ac:dyDescent="0.3">
       <c r="B57" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="10"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" s="10"/>
     </row>
-    <row r="62" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" ht="18" x14ac:dyDescent="0.3">
       <c r="B62" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="10"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="10"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="10"/>
     </row>
-    <row r="67" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B67" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="10"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="10"/>
     </row>
-    <row r="71" spans="2:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" ht="18" x14ac:dyDescent="0.3">
       <c r="B71" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" s="10"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="10"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="10"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" s="10"/>
     </row>
-    <row r="77" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B77" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="10"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="10"/>
     </row>
-    <row r="81" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B81" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="11"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="11"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="11"/>
     </row>
   </sheetData>
@@ -1628,13 +1662,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="88.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+    <col min="2" max="2" width="88.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -1642,12 +1676,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>101</v>
       </c>
@@ -1655,7 +1689,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>103</v>
       </c>
@@ -1663,7 +1697,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>105</v>
       </c>
@@ -1671,7 +1705,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>107</v>
       </c>
@@ -1679,7 +1713,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>109</v>
       </c>
@@ -1687,7 +1721,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>111</v>
       </c>
@@ -1695,7 +1729,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>113</v>
       </c>
@@ -1703,7 +1737,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>115</v>
       </c>
@@ -1711,29 +1745,29 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ml la 97, whizlabs 87, quizlet in prog.
</commit_message>
<xml_diff>
--- a/04-English/EN3-work.xlsx
+++ b/04-English/EN3-work.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t>too dire</t>
   </si>
@@ -473,6 +473,27 @@
   </si>
   <si>
     <t>text in a formal agreement that is printed smaller than the rest of the text, sometimes in the hope that it will not be noticed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inadvertently </t>
+  </si>
+  <si>
+    <t>veletlenul</t>
+  </si>
+  <si>
+    <t>intrinsically</t>
+  </si>
+  <si>
+    <t>eredendoen</t>
+  </si>
+  <si>
+    <t>is an essential or natural way / the attributed income will intrinsically influence the result more due to its larger value</t>
+  </si>
+  <si>
+    <t>labor</t>
+  </si>
+  <si>
+    <t>munkaero</t>
   </si>
 </sst>
 </file>
@@ -573,11 +594,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -885,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,6 +1200,33 @@
       </c>
       <c r="C33" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>152</v>
+      </c>
+      <c r="B35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
@@ -1378,7 +1426,7 @@
       <c r="A19" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1386,13 +1434,13 @@
       <c r="A20" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>130</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="11"/>
     </row>
     <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1403,18 +1451,18 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
+      <c r="B24" s="11"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
+      <c r="B25" s="11"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="12"/>
+      <c r="B26" s="11"/>
     </row>
     <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
@@ -1616,21 +1664,26 @@
       </c>
     </row>
     <row r="82" spans="2:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B83" s="11"/>
+      <c r="B83" s="12"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B84" s="11"/>
+      <c r="B84" s="12"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B85" s="11"/>
+      <c r="B85" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B63:B66"/>
     <mergeCell ref="B52:B56"/>
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="B2:B5"/>
@@ -1643,11 +1696,6 @@
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B63:B66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ml LA flashcards, 159-3-3-3
</commit_message>
<xml_diff>
--- a/04-English/EN3-work.xlsx
+++ b/04-English/EN3-work.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
   <si>
     <t>too dire</t>
   </si>
@@ -494,6 +494,42 @@
   </si>
   <si>
     <t>munkaero</t>
+  </si>
+  <si>
+    <t>residuals</t>
+  </si>
+  <si>
+    <t>maradekok</t>
+  </si>
+  <si>
+    <t>remedy</t>
+  </si>
+  <si>
+    <t>jogorvoslat, gyogyszer</t>
+  </si>
+  <si>
+    <t>subtle</t>
+  </si>
+  <si>
+    <t>apro, hajszalnyi, kifinomult</t>
+  </si>
+  <si>
+    <t>flatten</t>
+  </si>
+  <si>
+    <t>lelapul, lapit</t>
+  </si>
+  <si>
+    <t>scatter</t>
+  </si>
+  <si>
+    <t>szetszor, elterjeszt</t>
+  </si>
+  <si>
+    <t>damping factor</t>
+  </si>
+  <si>
+    <t>csillapito tenyezo</t>
   </si>
 </sst>
 </file>
@@ -907,7 +943,7 @@
   <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1227,6 +1263,54 @@
       </c>
       <c r="B36" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B41" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>167</v>
+      </c>
+      <c r="B42" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
apis and web services, blcokchain, spa
</commit_message>
<xml_diff>
--- a/04-English/EN3-work.xlsx
+++ b/04-English/EN3-work.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>too dire</t>
   </si>
@@ -605,6 +605,12 @@
   </si>
   <si>
     <t>RPA developer ?!</t>
+  </si>
+  <si>
+    <t>one-stop place</t>
+  </si>
+  <si>
+    <t>place capable of meeting all of the needs of its visitors or customers.</t>
   </si>
 </sst>
 </file>
@@ -705,11 +711,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1017,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,11 +1468,19 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>188</v>
+      </c>
       <c r="B51" t="s">
-        <v>188</v>
-      </c>
-      <c r="C51" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>194</v>
+      </c>
+      <c r="B52" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.25">
@@ -1533,7 +1547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -1666,7 +1680,7 @@
       <c r="A19" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1674,13 +1688,13 @@
       <c r="A20" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>130</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="11"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1694,7 +1708,7 @@
       <c r="A23" t="s">
         <v>190</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1702,19 +1716,19 @@
       <c r="A24" t="s">
         <v>191</v>
       </c>
-      <c r="B24" s="12"/>
+      <c r="B24" s="11"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>192</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="11"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>193</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="11"/>
     </row>
     <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
@@ -1916,21 +1930,26 @@
       </c>
     </row>
     <row r="82" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="11"/>
+      <c r="B83" s="12"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="11"/>
+      <c r="B84" s="12"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="11"/>
+      <c r="B85" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B82:B85"/>
+    <mergeCell ref="B63:B66"/>
     <mergeCell ref="B52:B56"/>
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="B2:B5"/>
@@ -1943,11 +1962,6 @@
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B82:B85"/>
-    <mergeCell ref="B63:B66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>